<commit_message>
update notebook and model
</commit_message>
<xml_diff>
--- a/models/model_results_table.xlsx
+++ b/models/model_results_table.xlsx
@@ -429,19 +429,19 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1.381</v>
+        <v>1.067</v>
       </c>
       <c r="C2">
-        <v>77.18000000000001</v>
+        <v>87.48999999999999</v>
       </c>
       <c r="D2">
-        <v>0.7888112307359588</v>
+        <v>0.8745349133623914</v>
       </c>
       <c r="E2">
-        <v>0.7717744316504281</v>
+        <v>0.8749138864285011</v>
       </c>
       <c r="F2">
-        <v>0.7465715156417052</v>
+        <v>0.8747007090139474</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -449,19 +449,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.321</v>
+        <v>0.847</v>
       </c>
       <c r="C3">
-        <v>70.86</v>
+        <v>83.36</v>
       </c>
       <c r="D3">
-        <v>0.770488052494064</v>
+        <v>0.8315504769193574</v>
       </c>
       <c r="E3">
-        <v>0.70859167404783</v>
+        <v>0.8335793721090444</v>
       </c>
       <c r="F3">
-        <v>0.6368748139016087</v>
+        <v>0.8302390533556168</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -469,19 +469,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.397</v>
+        <v>1.004</v>
       </c>
       <c r="C4">
-        <v>71.20999999999999</v>
+        <v>83.51000000000001</v>
       </c>
       <c r="D4">
-        <v>0.7782422169798308</v>
+        <v>0.8329853394489325</v>
       </c>
       <c r="E4">
-        <v>0.7121346324180691</v>
+        <v>0.8350556047633106</v>
       </c>
       <c r="F4">
-        <v>0.6418780091977716</v>
+        <v>0.8320270707161667</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -489,19 +489,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>40.804</v>
+        <v>92.075</v>
       </c>
       <c r="C5">
-        <v>79.13</v>
+        <v>86.22</v>
       </c>
       <c r="D5">
-        <v>0.7927917253939653</v>
+        <v>0.8609613235349567</v>
       </c>
       <c r="E5">
-        <v>0.7912607026867434</v>
+        <v>0.8622182856018108</v>
       </c>
       <c r="F5">
-        <v>0.7789155694733482</v>
+        <v>0.8611804373832499</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -509,19 +509,19 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>49.139</v>
+        <v>11.072</v>
       </c>
       <c r="C6">
-        <v>77.90000000000001</v>
+        <v>87.5</v>
       </c>
       <c r="D6">
-        <v>0.7853185353628601</v>
+        <v>0.8741952150343126</v>
       </c>
       <c r="E6">
-        <v>0.7789587639011908</v>
+        <v>0.8750123019387855</v>
       </c>
       <c r="F6">
-        <v>0.7609806031311999</v>
+        <v>0.8744435692318999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>